<commit_message>
Capturados nuevas celdas en cada tipo de archivo
</commit_message>
<xml_diff>
--- a/dist/outputs/Ica-Estructurado.xlsx
+++ b/dist/outputs/Ica-Estructurado.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Concepto</t>
   </si>
@@ -28,10 +28,19 @@
     <t>Razón Social</t>
   </si>
   <si>
+    <t>Bimestre o Período Anual</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Anual</t>
+  </si>
+  <si>
+    <t>INVERSIONES ORTIZ VASQUEZ HERMANOS S A S</t>
+  </si>
+  <si>
     <t>TOTAL INGRESOS ORDINARIOS Y EXTRAORDINARIOS DEL PERIODO EN TODO EL PAIS</t>
-  </si>
-  <si>
-    <t>INVERSIONES ORTIZ VASQUEZ HERMANOS S A S</t>
   </si>
   <si>
     <t>MENOS INGRESOS FUERA DE ESTE MUNICIPIO O DISTRITO</t>
@@ -180,7 +189,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -209,7 +218,7 @@
     </row>
     <row r="2" spans="1:5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>8</v>
@@ -221,12 +230,12 @@
         <v>2019</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>9</v>
@@ -238,12 +247,12 @@
         <v>2019</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>10</v>
@@ -255,12 +264,12 @@
         <v>2019</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>11</v>
@@ -272,12 +281,12 @@
         <v>2019</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>12</v>
@@ -289,12 +298,12 @@
         <v>2019</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>13</v>
@@ -306,12 +315,12 @@
         <v>2019</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>14</v>
@@ -323,12 +332,12 @@
         <v>2019</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>15</v>
@@ -340,12 +349,12 @@
         <v>2019</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>16</v>
@@ -357,12 +366,12 @@
         <v>2019</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>17</v>
@@ -374,12 +383,12 @@
         <v>2019</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>18</v>
@@ -391,12 +400,12 @@
         <v>2019</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>19</v>
@@ -408,12 +417,12 @@
         <v>2019</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>20</v>
@@ -425,12 +434,12 @@
         <v>2019</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>21</v>
@@ -442,12 +451,12 @@
         <v>2019</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>22</v>
@@ -459,12 +468,12 @@
         <v>2019</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>23</v>
@@ -476,12 +485,12 @@
         <v>2019</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>24</v>
@@ -493,12 +502,12 @@
         <v>2019</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>25</v>
@@ -510,12 +519,12 @@
         <v>2019</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>26</v>
@@ -527,12 +536,12 @@
         <v>2019</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>27</v>
@@ -544,12 +553,12 @@
         <v>2019</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>28</v>
@@ -561,12 +570,12 @@
         <v>2019</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>29</v>
@@ -578,12 +587,12 @@
         <v>2019</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>30</v>
@@ -595,12 +604,12 @@
         <v>2019</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>31</v>
@@ -612,12 +621,12 @@
         <v>2019</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>32</v>
@@ -629,12 +638,12 @@
         <v>2019</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>33</v>
@@ -646,12 +655,12 @@
         <v>2019</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>34</v>
@@ -663,12 +672,12 @@
         <v>2019</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>35</v>
@@ -680,12 +689,12 @@
         <v>2019</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>36</v>
@@ -697,12 +706,12 @@
         <v>2019</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>37</v>
@@ -714,12 +723,12 @@
         <v>2019</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:5" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>38</v>
@@ -731,12 +740,12 @@
         <v>2019</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:5" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>39</v>
@@ -748,12 +757,12 @@
         <v>2019</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:5" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>40</v>
@@ -765,7 +774,24 @@
         <v>2019</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" customHeight="1">
+      <c r="A35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>